<commit_message>
working 2nd analytic trail
working 2nd analytic trail.
</commit_message>
<xml_diff>
--- a/data/health/indicator_1 gapminder infant_mortality.xlsx
+++ b/data/health/indicator_1 gapminder infant_mortality.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21140" windowWidth="38400" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-21140" windowWidth="19200" windowHeight="21140" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="65">
   <si>
     <t>No footnotes</t>
   </si>
@@ -221,6 +221,12 @@
   </si>
   <si>
     <t>Zimbabwe</t>
+  </si>
+  <si>
+    <t>Hong Kong</t>
+  </si>
+  <si>
+    <t>South Korea</t>
   </si>
 </sst>
 </file>
@@ -881,7 +887,7 @@
   <dimension ref="A1:H768"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+      <selection activeCell="B2" sqref="B2:H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1126,544 +1132,536 @@
       </c>
     </row>
     <row r="10" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="13" t="s">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B11" s="18">
         <v>103.1</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C11" s="18">
         <v>90.7</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D11" s="18">
         <v>79.599999999999994</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E11" s="18">
         <v>68.599999999999994</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F11" s="18">
         <v>57.8</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G11" s="4">
         <v>48.2</v>
       </c>
-      <c r="H10" s="12">
+      <c r="H11" s="12">
         <v>39.299999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="13" t="s">
+    <row r="12" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B12" s="18">
         <v>5.8</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C12" s="18">
         <v>4.7</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D12" s="18">
         <v>4.3</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E12" s="18">
         <v>3.4</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F12" s="18">
         <v>2.9</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G12" s="4">
         <v>2.4</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H12" s="12">
         <v>2.1</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="13" t="s">
+    <row r="13" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B13" s="18">
         <v>51.4</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C13" s="18">
         <v>45.2</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D13" s="18">
         <v>45</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E13" s="18">
         <v>39.4</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F13" s="18">
         <v>30.3</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G13" s="4">
         <v>21.1</v>
       </c>
-      <c r="H12" s="12">
+      <c r="H13" s="12">
         <v>13.5</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="13" t="s">
+    <row r="14" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B14" s="4">
         <v>35</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C14" s="4">
         <v>28.2</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D14" s="18">
         <v>22.7</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E14" s="18">
         <v>18.100000000000001</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F14" s="18">
         <v>13.1</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G14" s="4">
         <v>9.1999999999999993</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H14" s="12">
         <v>7.3</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="13" t="s">
+    <row r="15" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B15" s="18">
         <v>19.7</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C15" s="18">
         <v>15</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D15" s="18">
         <v>11.9</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E15" s="18">
         <v>9.4</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F15" s="18">
         <v>7.1</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G15" s="4">
         <v>6.9</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H15" s="12">
         <v>6.2</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="13" t="s">
+    <row r="16" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="18">
+      <c r="B16" s="18">
         <v>47.3</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C16" s="18">
         <v>38.799999999999997</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D16" s="18">
         <v>30.4</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E16" s="18">
         <v>22.9</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F16" s="18">
         <v>17.399999999999999</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G16" s="4">
         <v>15</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H16" s="12">
         <v>11.9</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="13" t="s">
+    <row r="17" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B17" s="4">
         <v>8</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C17" s="4">
         <v>7</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D17" s="18">
         <v>5.8</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E17" s="18">
         <v>5.2</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F17" s="18">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G17" s="4">
         <v>3.8</v>
       </c>
-      <c r="H16" s="12">
+      <c r="H17" s="12">
         <v>3.3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="13" t="s">
+    <row r="18" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B18" s="4">
         <v>11.6</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C18" s="4">
         <v>9.6999999999999993</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D18" s="4">
         <v>7.5</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E18" s="4">
         <v>6.2</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F18" s="4">
         <v>5.5</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G18" s="4">
         <v>5.2</v>
       </c>
-      <c r="H17" s="12">
+      <c r="H18" s="12">
         <v>4.8</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="13" t="s">
+    <row r="19" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B19" s="18">
         <v>116.4</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C19" s="18">
         <v>107.8</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D19" s="18">
         <v>98.9</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E19" s="18">
         <v>89.5</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F19" s="18">
         <v>81.400000000000006</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G19" s="4">
         <v>74.8</v>
       </c>
-      <c r="H18" s="12">
+      <c r="H19" s="12">
         <v>67.400000000000006</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="13" t="s">
+    <row r="20" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="18">
+      <c r="B20" s="18">
         <v>50.9</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C20" s="18">
         <v>42.8</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D20" s="18">
         <v>34.6</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E20" s="18">
         <v>30.5</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F20" s="18">
         <v>27.9</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G20" s="4">
         <v>25.4</v>
       </c>
-      <c r="H19" s="12">
+      <c r="H20" s="12">
         <v>22.8</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="13" t="s">
+    <row r="21" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="18">
+      <c r="B21" s="18">
         <v>18.600000000000001</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C21" s="18">
         <v>15.7</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D21" s="18">
         <v>13.5</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E21" s="18">
         <v>8.6</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F21" s="18">
         <v>6.7</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G21" s="4">
         <v>5.3</v>
       </c>
-      <c r="H20" s="12">
+      <c r="H21" s="12">
         <v>4.5</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="13" t="s">
+    <row r="22" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="18">
+      <c r="B22" s="18">
         <v>31.6</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C22" s="18">
         <v>32</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D22" s="18">
         <v>27.9</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E22" s="18">
         <v>24.2</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F22" s="18">
         <v>19.5</v>
       </c>
-      <c r="G21" s="4">
+      <c r="G22" s="4">
         <v>13</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H22" s="12">
         <v>10.1</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="13" t="s">
+    <row r="23" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B23" s="4">
         <v>25.6</v>
       </c>
-      <c r="C22" s="4">
+      <c r="C23" s="4">
         <v>22.2</v>
       </c>
-      <c r="D22" s="4">
+      <c r="D23" s="4">
         <v>22.2</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E23" s="4">
         <v>20.5</v>
       </c>
-      <c r="F22" s="4">
+      <c r="F23" s="4">
         <v>15.4</v>
       </c>
-      <c r="G22" s="4">
+      <c r="G23" s="4">
         <v>10.9</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H23" s="12">
         <v>8.5</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="13" t="s">
+    <row r="24" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="18">
+      <c r="B24" s="18">
         <v>9.4</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C24" s="18">
         <v>6.7</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D24" s="18">
         <v>4.3</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E24" s="18">
         <v>3.4</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F24" s="18">
         <v>2.2999999999999998</v>
       </c>
-      <c r="G23" s="4">
+      <c r="G24" s="4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="H23" s="12">
+      <c r="H24" s="12">
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="13" t="s">
+    <row r="25" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="18">
+      <c r="B26" s="18">
         <v>12</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C26" s="18">
         <v>9.6999999999999993</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D26" s="18">
         <v>7.5</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E26" s="18">
         <v>5.6</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F26" s="18">
         <v>5</v>
       </c>
-      <c r="G24" s="4">
+      <c r="G26" s="4">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H24" s="12">
+      <c r="H26" s="12">
         <v>3.6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="13" t="s">
+    <row r="27" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B27" s="4">
         <v>6.5</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C27" s="4">
         <v>6.1</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D27" s="4">
         <v>4.4000000000000004</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E27" s="4">
         <v>3.4</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F27" s="4">
         <v>3.1</v>
       </c>
-      <c r="G25" s="4">
+      <c r="G27" s="4">
         <v>2.5</v>
       </c>
-      <c r="H25" s="12">
+      <c r="H27" s="12">
         <v>2.4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="13" t="s">
+    <row r="28" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B28" s="18">
         <v>7</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C28" s="18">
         <v>6</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D28" s="18">
         <v>5</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E28" s="18">
         <v>7</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F28" s="18">
         <v>6</v>
       </c>
-      <c r="G26" s="4">
+      <c r="G28" s="4">
         <v>6</v>
       </c>
-      <c r="H26" s="12">
+      <c r="H28" s="12">
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="13" t="s">
+    <row r="29" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B29" s="18">
         <v>40</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C29" s="18">
         <v>31.9</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D29" s="18">
         <v>24.8</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E29" s="18">
         <v>19.899999999999999</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F29" s="18">
         <v>16</v>
       </c>
-      <c r="G27" s="4">
+      <c r="G29" s="4">
         <v>12.9</v>
       </c>
-      <c r="H27" s="12">
+      <c r="H29" s="12">
         <v>10.9</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="13" t="s">
+    <row r="30" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="18">
+      <c r="B30" s="18">
         <v>10.9</v>
       </c>
-      <c r="C28" s="18">
+      <c r="C30" s="18">
         <v>9.6999999999999993</v>
       </c>
-      <c r="D28" s="18">
+      <c r="D30" s="18">
         <v>8.1999999999999993</v>
       </c>
-      <c r="E28" s="18">
+      <c r="E30" s="18">
         <v>7.2</v>
       </c>
-      <c r="F28" s="18">
+      <c r="F30" s="18">
         <v>6.9</v>
       </c>
-      <c r="G28" s="4">
+      <c r="G30" s="4">
         <v>6.4</v>
       </c>
-      <c r="H28" s="12">
+      <c r="H30" s="12">
         <v>5.7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="13" t="s">
+    <row r="31" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="B29" s="31">
+      <c r="B31" s="31">
         <v>56</v>
       </c>
-      <c r="C29" s="31">
+      <c r="C31" s="31">
         <v>50.2</v>
       </c>
-      <c r="D29" s="4">
+      <c r="D31" s="4">
         <v>58.1</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E31" s="4">
         <v>63.5</v>
       </c>
-      <c r="F29" s="4">
+      <c r="F31" s="4">
         <v>61.5</v>
       </c>
-      <c r="G29" s="4">
+      <c r="G31" s="4">
         <v>57.7</v>
       </c>
-      <c r="H29" s="12">
+      <c r="H31" s="12">
         <v>47.6</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="13"/>
-      <c r="B30" s="4"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-    </row>
-    <row r="31" spans="1:8" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-    </row>
-    <row r="32" spans="1:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -1672,7 +1670,7 @@
       <c r="F32" s="12"/>
       <c r="G32" s="12"/>
     </row>
-    <row r="33" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:7" ht="14" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>

</xml_diff>